<commit_message>
Alta plan de estudio
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCases.xlsx
+++ b/src/main/resources/TestCases.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="100">
   <si>
     <t>id</t>
   </si>
@@ -96,34 +96,28 @@
     <t>login</t>
   </si>
   <si>
-    <t>FerDearrasca@mail.com</t>
+    <t>automation3@test.com</t>
   </si>
   <si>
     <t>1234</t>
   </si>
   <si>
-    <t>2</t>
+    <t>9</t>
   </si>
   <si>
-    <t>altaCarrera</t>
+    <t>agregarPlanEstudio</t>
   </si>
   <si>
-    <t>x</t>
+    <t>&lt;empty&gt;</t>
   </si>
   <si>
-    <t>carrera 1</t>
+    <t>c2</t>
   </si>
   <si>
-    <t>lorem ipsum sit amen</t>
+    <t>asignatura0001:1;asignatura0002:2</t>
   </si>
   <si>
     <t>s</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>logout</t>
   </si>
   <si>
     <t>PedroPeAdmin@mail.com</t>
@@ -150,6 +144,18 @@
     <t>funcionario1</t>
   </si>
   <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>altaCarrera</t>
+  </si>
+  <si>
+    <t>carrera 1</t>
+  </si>
+  <si>
+    <t>lorem ipsum sit amen</t>
+  </si>
+  <si>
     <t>altaAsignatura</t>
   </si>
   <si>
@@ -160,9 +166,6 @@
   </si>
   <si>
     <t>asignatura 2</t>
-  </si>
-  <si>
-    <t>agregarPlanEstudio</t>
   </si>
   <si>
     <t>asignatura 1:1;asignatura 2:2</t>
@@ -279,10 +282,55 @@
     <t>El usuario no logró iniciar sesión y recibió el mensaje de error correspondiente.</t>
   </si>
   <si>
-    <t>Alta de usuarios coordinadores y funcionarios</t>
+    <t>Alta de usuarios coordinadores</t>
   </si>
   <si>
     <t>El usuario administrador da de alta a un usuario coordinador.</t>
+  </si>
+  <si>
+    <t>Estar logueado como un usuario administrador.</t>
+  </si>
+  <si>
+    <t>Nombre:Coordinador
+Apellido:Doe
+Email:email@gmail.com
+CI:12345678
+Fecha Nacimiento:1/1/1999
+Direccion:Direccion
+Telefono:099999998
+Tipo Usuario:COORDINADOR
+Contraseña:1234
+Confirmacion Contraseña:1234</t>
+  </si>
+  <si>
+    <t>1- El usuario hace click en el apartado Usuarios.
+2- El usuario hace click en el botón Agregar Usuario.
+3- El usuario completa los campos con los datos correspondientes.
+4- El usuario hace click en el botón Agregar.</t>
+  </si>
+  <si>
+    <t>El usuario es dado de alta correctamente.</t>
+  </si>
+  <si>
+    <t>El usuario es dado de alta correctamente devolviendo al administrador a la pantalla con la lista de usuarios con el usuario nuevo en ella.</t>
+  </si>
+  <si>
+    <t>Alta de usuarios funcionarios</t>
+  </si>
+  <si>
+    <t>El usuario administrador da de alta a un usuario funcionario.</t>
+  </si>
+  <si>
+    <t>Nombre:Funcionario
+Apellido:Doe
+Email:email@gmail.com
+CI:12345678
+Fecha Nacimiento:1/1/1999
+Direccion:Direccion
+Telefono:099999998
+Tipo Usuario:FUNCIONARIO
+Contraseña:1234
+Confirmacion Contraseña:1234</t>
   </si>
   <si>
     <t>Desactivar cuenta de usuario
@@ -334,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -365,13 +413,16 @@
       <alignment shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,9 +649,11 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="3" width="20.63"/>
+    <col customWidth="1" min="5" max="5" width="17.25"/>
     <col customWidth="1" min="11" max="11" width="13.63"/>
     <col customWidth="1" min="13" max="13" width="16.88"/>
     <col customWidth="1" min="14" max="14" width="14.63"/>
+    <col customWidth="1" min="19" max="19" width="27.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -769,19 +822,31 @@
         <v>32</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
       <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
       <c r="Y3" s="1" t="s">
         <v>34</v>
       </c>
@@ -795,12 +860,8 @@
       <c r="AG3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -823,9 +884,7 @@
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
-      <c r="Y4" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="Y4" s="1"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
@@ -35707,7 +35766,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" s="3">
         <v>1234.0</v>
@@ -35721,16 +35780,16 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3">
         <v>1234.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>5</v>
@@ -35742,13 +35801,13 @@
         <v>36526.0</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J3" s="4">
         <v>9.5111222E7</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Y3" s="3" t="s">
         <v>34</v>
@@ -35759,16 +35818,16 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4" s="3">
         <v>1234.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>5</v>
@@ -35780,13 +35839,13 @@
         <v>36526.0</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J4" s="4">
         <v>9.5111222E7</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Y4" s="3" t="s">
         <v>34</v>
@@ -35797,7 +35856,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="Y5" s="3" t="s">
         <v>34</v>
@@ -35811,7 +35870,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" s="3">
         <v>1234.0</v>
@@ -35825,13 +35884,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="Y7" s="3" t="s">
         <v>34</v>
@@ -35842,13 +35901,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -35864,13 +35923,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
@@ -35886,10 +35945,10 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U10" s="5"/>
       <c r="V10" s="3"/>
@@ -35904,10 +35963,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
@@ -35920,7 +35979,7 @@
         <v>45504.0</v>
       </c>
       <c r="V11" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="W11" s="6">
         <v>0.4166666666666667</v>
@@ -35937,10 +35996,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
@@ -35953,7 +36012,7 @@
         <v>45504.0</v>
       </c>
       <c r="V12" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="W12" s="6">
         <v>0.375</v>
@@ -35970,10 +36029,10 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="P13" s="3"/>
       <c r="Q13" s="5">
@@ -35994,7 +36053,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="N14" s="3"/>
       <c r="P14" s="3"/>
@@ -36016,7 +36075,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D15" s="3">
         <v>1234.0</v>
@@ -36038,13 +36097,13 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
@@ -36061,7 +36120,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="Y17" s="3" t="s">
         <v>34</v>
@@ -36072,19 +36131,19 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D18" s="3">
         <v>1234.0</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G18" s="3">
         <v>1.1112223E7</v>
@@ -36093,7 +36152,7 @@
         <v>36526.0</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J18" s="3">
         <v>1.11222333E8</v>
@@ -36110,7 +36169,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D19" s="3">
         <v>1234.0</v>
@@ -36124,10 +36183,10 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Y20" s="3" t="s">
         <v>34</v>
@@ -36138,7 +36197,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="Y21" s="3" t="s">
         <v>34</v>
@@ -36152,7 +36211,7 @@
         <v>26</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D22" s="3">
         <v>1234.0</v>
@@ -36166,16 +36225,16 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Y23" s="3" t="s">
         <v>34</v>
@@ -36186,7 +36245,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="Y24" s="3" t="s">
         <v>34</v>
@@ -36200,7 +36259,7 @@
         <v>26</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D25" s="3">
         <v>1234.0</v>
@@ -36214,10 +36273,10 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Y26" s="3" t="s">
         <v>34</v>
@@ -36228,10 +36287,10 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Y27" s="3" t="s">
         <v>34</v>
@@ -36286,10 +36345,10 @@
     <col customWidth="1" min="2" max="2" width="33.0"/>
     <col customWidth="1" min="3" max="3" width="27.25"/>
     <col customWidth="1" min="4" max="4" width="20.5"/>
-    <col customWidth="1" min="5" max="5" width="22.25"/>
+    <col customWidth="1" min="5" max="5" width="29.38"/>
     <col customWidth="1" min="6" max="6" width="35.63"/>
     <col customWidth="1" min="7" max="7" width="22.88"/>
-    <col customWidth="1" min="8" max="8" width="20.5"/>
+    <col customWidth="1" min="8" max="8" width="21.75"/>
     <col customWidth="1" min="9" max="9" width="21.88"/>
     <col customWidth="1" min="10" max="10" width="29.25"/>
     <col customWidth="1" min="11" max="11" width="13.63"/>
@@ -36300,39 +36359,39 @@
     <col customWidth="1" min="23" max="24" width="8.25"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="18.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="2" ht="69.75" customHeight="1">
+    <row r="2" ht="80.25" customHeight="1">
       <c r="A2" s="7">
         <v>1.0</v>
       </c>
@@ -36340,31 +36399,31 @@
         <v>26</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
     </row>
-    <row r="3">
+    <row r="3" ht="71.25" customHeight="1">
       <c r="A3" s="7">
         <v>2.0</v>
       </c>
@@ -36372,64 +36431,90 @@
         <v>26</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" ht="63.75" customHeight="1">
+    <row r="4" ht="126.75" customHeight="1">
       <c r="A4" s="7">
         <v>3.0</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="10"/>
+      <c r="D4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
     </row>
-    <row r="5" ht="35.25" customHeight="1">
+    <row r="5" ht="126.0" customHeight="1">
       <c r="A5" s="7">
         <v>4.0</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="C5" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
@@ -36438,11 +36523,13 @@
       <c r="A6" s="7">
         <v>5.0</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>88</v>
+      <c r="B6" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
+      <c r="D6" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -36456,11 +36543,13 @@
       <c r="A7" s="7">
         <v>6.0</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -36474,11 +36563,13 @@
       <c r="A8" s="7">
         <v>7.0</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>90</v>
+      <c r="B8" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
+      <c r="D8" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -36652,7 +36743,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="12"/>
+      <c r="H18" s="14"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>

</xml_diff>